<commit_message>
Add test result columns
</commit_message>
<xml_diff>
--- a/xxetest/Java XXE Test Case Results.xlsx
+++ b/xxetest/Java XXE Test Case Results.xlsx
@@ -1,26 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwichers/git/security-unit-tests/xxetest/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="24820" windowHeight="15540"/>
+    <workbookView xWindow="780" yWindow="465" windowWidth="24825" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Java XXE Unit Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Fortify Results" sheetId="2" r:id="rId2"/>
     <sheet name="Contrast Results" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="107">
   <si>
     <t>Filename</t>
   </si>
@@ -171,22 +163,6 @@
   </si>
   <si>
     <r>
-      <t>javax.xml.parsers.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DocumentBuilder</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>javax.xml.bind.</t>
     </r>
     <r>
@@ -437,22 +413,36 @@
   <si>
     <t>XXE Tests</t>
   </si>
+  <si>
+    <t>Fortify Detection</t>
+  </si>
+  <si>
+    <t>Contrast Detection</t>
+  </si>
+  <si>
+    <t>javax.xml.parsers.DocumentBuilder</t>
+  </si>
+  <si>
+    <t>Unsafe (Safe in 1.8)</t>
+  </si>
+  <si>
+    <t>Fail (Pass in 1.8)</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -466,15 +456,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -489,13 +478,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -521,32 +510,452 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Total" xfId="2" builtinId="25"/>
+    <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="54">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -631,7 +1040,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.404761904761905</c:v>
+                  <c:v>0.40476190476190471</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -643,7 +1052,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.857142857142857</c:v>
+                  <c:v>0.8571428571428571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -679,10 +1088,10 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="2"/>
               <c:pt idx="0">
-                <c:v>0.0</c:v>
+                <c:v>0</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:xVal>
@@ -691,10 +1100,10 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="2"/>
               <c:pt idx="0">
-                <c:v>0.0</c:v>
+                <c:v>0</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:yVal>
@@ -708,15 +1117,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1099509168"/>
-        <c:axId val="1099512560"/>
+        <c:axId val="43966464"/>
+        <c:axId val="43967040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1099509168"/>
+        <c:axId val="43966464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -749,17 +1158,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1099512560"/>
+        <c:crossAx val="43967040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1099512560"/>
+        <c:axId val="43967040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -787,7 +1196,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1099509168"/>
+        <c:crossAx val="43966464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -843,7 +1252,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.33333333333333337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -855,7 +1264,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.857142857142857</c:v>
+                  <c:v>0.8571428571428571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -891,10 +1300,10 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="2"/>
               <c:pt idx="0">
-                <c:v>0.0</c:v>
+                <c:v>0</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:xVal>
@@ -903,10 +1312,10 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="2"/>
               <c:pt idx="0">
-                <c:v>0.0</c:v>
+                <c:v>0</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:yVal>
@@ -920,15 +1329,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1099538080"/>
-        <c:axId val="1099541472"/>
+        <c:axId val="43968768"/>
+        <c:axId val="43969344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1099538080"/>
+        <c:axId val="43968768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -961,17 +1370,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1099541472"/>
+        <c:crossAx val="43969344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1099541472"/>
+        <c:axId val="43969344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -999,7 +1408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1099538080"/>
+        <c:crossAx val="43968768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1055,7 +1464,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.0714285714285714</c:v>
+                  <c:v>7.1428571428571425E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1067,7 +1476,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1103,10 +1512,10 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="2"/>
               <c:pt idx="0">
-                <c:v>0.0</c:v>
+                <c:v>0</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:xVal>
@@ -1115,10 +1524,10 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="2"/>
               <c:pt idx="0">
-                <c:v>0.0</c:v>
+                <c:v>0</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:yVal>
@@ -1132,15 +1541,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1014699136"/>
-        <c:axId val="1014126320"/>
+        <c:axId val="43971648"/>
+        <c:axId val="43972224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1014699136"/>
+        <c:axId val="43971648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1173,17 +1582,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1014126320"/>
+        <c:crossAx val="43972224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1014126320"/>
+        <c:axId val="43972224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1211,7 +1620,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1014699136"/>
+        <c:crossAx val="43971648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1334,14 +1743,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F40">
-  <autoFilter ref="A1:F40"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H40">
+  <autoFilter ref="A1:H40"/>
+  <tableColumns count="8">
     <tableColumn id="8" name="XXE Tests"/>
     <tableColumn id="3" name="XML Parser" totalsRowLabel="Total"/>
     <tableColumn id="1" name="Filename"/>
     <tableColumn id="6" name="Method"/>
     <tableColumn id="5" name="Testing if…"/>
+    <tableColumn id="4" name="Fortify Detection"/>
+    <tableColumn id="7" name="Contrast Detection"/>
     <tableColumn id="2" name="Test Description" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1357,10 +1768,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="11"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="10"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="9"/>
-    <tableColumn id="9" name="Score" dataDxfId="8"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="53"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="52"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="51"/>
+    <tableColumn id="9" name="Score" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1375,10 +1786,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="7"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="6"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="5"/>
-    <tableColumn id="9" name="Score" dataDxfId="4"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="49"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="48"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="47"/>
+    <tableColumn id="9" name="Score" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1393,10 +1804,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="3"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="2"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="1"/>
-    <tableColumn id="9" name="Score" dataDxfId="0"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="45"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="44"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="43"/>
+    <tableColumn id="9" name="Score" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1689,26 +2100,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="141.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="141.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>100</v>
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -1719,16 +2131,22 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1743,12 +2161,18 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1763,12 +2187,18 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1783,10 +2213,16 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="G4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1803,30 +2239,42 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1843,10 +2291,16 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1863,10 +2317,16 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1883,10 +2343,16 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1903,10 +2369,16 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1923,15 +2395,21 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1940,18 +2418,24 @@
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="G12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1963,15 +2447,21 @@
         <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1983,15 +2473,21 @@
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -2003,15 +2499,21 @@
         <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -2023,15 +2525,21 @@
         <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -2043,15 +2551,21 @@
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -2063,15 +2577,21 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G18" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2083,15 +2603,21 @@
         <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G19" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -2103,15 +2629,21 @@
         <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2123,15 +2655,21 @@
         <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G21" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -2143,15 +2681,21 @@
         <v>21</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="G22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -2163,35 +2707,47 @@
         <v>22</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -2203,15 +2759,21 @@
         <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -2223,15 +2785,21 @@
         <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="G26" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -2243,15 +2811,21 @@
         <v>22</v>
       </c>
       <c r="F27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -2263,15 +2837,21 @@
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="G28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -2283,15 +2863,21 @@
         <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -2303,15 +2889,21 @@
         <v>22</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="G30" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -2323,15 +2915,21 @@
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="G31" t="s">
+        <v>98</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
@@ -2343,15 +2941,21 @@
         <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G32" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
         <v>39</v>
@@ -2363,15 +2967,21 @@
         <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G33" t="s">
+        <v>105</v>
+      </c>
+      <c r="H33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
         <v>39</v>
@@ -2383,15 +2993,21 @@
         <v>21</v>
       </c>
       <c r="F34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
         <v>40</v>
@@ -2403,15 +3019,21 @@
         <v>22</v>
       </c>
       <c r="F35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G35" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -2423,15 +3045,21 @@
         <v>21</v>
       </c>
       <c r="F36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G36" t="s">
+        <v>105</v>
+      </c>
+      <c r="H36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
         <v>3</v>
@@ -2443,15 +3071,21 @@
         <v>22</v>
       </c>
       <c r="F37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G37" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
@@ -2463,15 +3097,21 @@
         <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G38" t="s">
+        <v>105</v>
+      </c>
+      <c r="H38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -2483,15 +3123,21 @@
         <v>22</v>
       </c>
       <c r="F39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="G39" t="s">
+        <v>106</v>
+      </c>
+      <c r="H39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -2503,10 +3149,32 @@
         <v>21</v>
       </c>
       <c r="F40" t="s">
-        <v>84</v>
+        <v>106</v>
+      </c>
+      <c r="G40" t="s">
+        <v>105</v>
+      </c>
+      <c r="H40" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Safe">
+      <formula>NOT(ISERROR(SEARCH("Safe",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="Unsafe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -2523,26 +3191,26 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2558,28 +3226,28 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>93</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>94</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>95</v>
-      </c>
-      <c r="I2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2589,7 +3257,7 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3"/>
       <c r="D3">
         <v>1</v>
       </c>
@@ -2600,27 +3268,27 @@
         <f t="shared" ref="F3:F9" si="0">SUM(B3:E3)</f>
         <v>7</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <f>IF(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]=0,"N/A",Table136[[#This Row],[True Positive]]/(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f>Table136[[#This Row],[False Positive]]/(Table136[[#This Row],[False Positive]]+Table136[[#This Row],[True Negative]])</f>
         <v>0.5</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <f>(Table136[[#This Row],[True Posistive Rate]]+(1 - Table136[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="4"/>
       <c r="D4">
         <v>1</v>
       </c>
@@ -2631,27 +3299,27 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f>IF(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]=0,"N/A",Table136[[#This Row],[True Positive]]/(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <f>Table136[[#This Row],[False Positive]]/(Table136[[#This Row],[False Positive]]+Table136[[#This Row],[True Negative]])</f>
         <v>0.5</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <f>(Table136[[#This Row],[True Posistive Rate]]+(1 - Table136[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
       <c r="D5">
         <v>2</v>
       </c>
@@ -2659,22 +3327,22 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f>IF(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]=0,"N/A",Table136[[#This Row],[True Positive]]/(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f>Table136[[#This Row],[False Positive]]/(Table136[[#This Row],[False Positive]]+Table136[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <f>(Table136[[#This Row],[True Posistive Rate]]+(1 - Table136[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2686,27 +3354,27 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f>IF(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]=0,"N/A",Table136[[#This Row],[True Positive]]/(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f>Table136[[#This Row],[False Positive]]/(Table136[[#This Row],[False Positive]]+Table136[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <f>(Table136[[#This Row],[True Posistive Rate]]+(1 - Table136[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
       <c r="E7">
         <v>2</v>
       </c>
@@ -2714,27 +3382,27 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f>IF(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]=0,"N/A",Table136[[#This Row],[True Positive]]/(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f>Table136[[#This Row],[False Positive]]/(Table136[[#This Row],[False Positive]]+Table136[[#This Row],[True Negative]])</f>
         <v>1</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <f>(Table136[[#This Row],[True Posistive Rate]]+(1 - Table136[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="4"/>
       <c r="D8">
         <v>2</v>
       </c>
@@ -2745,27 +3413,27 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f>IF(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]=0,"N/A",Table136[[#This Row],[True Positive]]/(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f>Table136[[#This Row],[False Positive]]/(Table136[[#This Row],[False Positive]]+Table136[[#This Row],[True Negative]])</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <f>(Table136[[#This Row],[True Posistive Rate]]+(1 - Table136[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
       <c r="D9">
         <v>2</v>
       </c>
@@ -2773,60 +3441,60 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f>IF(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]=0,"N/A",Table136[[#This Row],[True Positive]]/(Table136[[#This Row],[True Positive]]+Table136[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f>Table136[[#This Row],[False Positive]]/(Table136[[#This Row],[False Positive]]+Table136[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <f>(Table136[[#This Row],[True Posistive Rate]]+(1 - Table136[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="8">
+    <row r="10" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="7">
         <f t="shared" ref="B10" si="1">SUM(B3:B9)</f>
         <v>18</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <f t="shared" ref="C10" si="2">SUM(C3:C9)</f>
         <v>1</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <f t="shared" ref="D10" si="3">SUM(D3:D9)</f>
         <v>10</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <f t="shared" ref="E10" si="4">SUM(E3:E9)</f>
         <v>5</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <f>SUM(F3:F9)</f>
         <v>34</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f>AVERAGE(G3:G9)</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" ref="H10" si="5">AVERAGE(H3:H9)</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <f>ROUND(AVERAGE(I3:I9)*100, 0)</f>
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" ht="15.95" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -2837,36 +3505,36 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
         <v>89</v>
       </c>
-      <c r="C29" t="s">
+      <c r="F29" t="s">
         <v>92</v>
       </c>
-      <c r="D29" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>93</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>94</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>95</v>
       </c>
-      <c r="I29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2883,22 +3551,22 @@
         <f t="shared" ref="F30:F36" si="6">SUM(B30:E30)</f>
         <v>7</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="5">
         <f>IF(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]=0,"N/A",Table13[[#This Row],[True Positive]]/(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="5">
         <f>Table13[[#This Row],[False Positive]]/(Table13[[#This Row],[False Positive]]+Table13[[#This Row],[True Negative]])</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="5">
         <f>(Table13[[#This Row],[True Posistive Rate]]+(1 - Table13[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0.33333333333333348</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2910,22 +3578,22 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="5">
         <f>IF(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]=0,"N/A",Table13[[#This Row],[True Positive]]/(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="5">
         <f>Table13[[#This Row],[False Positive]]/(Table13[[#This Row],[False Positive]]+Table13[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31" s="5">
         <f>(Table13[[#This Row],[True Posistive Rate]]+(1 - Table13[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32">
         <v>5</v>
@@ -2940,22 +3608,22 @@
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="5">
         <f>IF(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]=0,"N/A",Table13[[#This Row],[True Positive]]/(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="5">
         <f>Table13[[#This Row],[False Positive]]/(Table13[[#This Row],[False Positive]]+Table13[[#This Row],[True Negative]])</f>
         <v>0.5</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="5">
         <f>(Table13[[#This Row],[True Posistive Rate]]+(1 - Table13[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -2967,22 +3635,22 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="5">
         <f>IF(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]=0,"N/A",Table13[[#This Row],[True Positive]]/(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H33" s="5">
         <f>Table13[[#This Row],[False Positive]]/(Table13[[#This Row],[False Positive]]+Table13[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33" s="5">
         <f>(Table13[[#This Row],[True Posistive Rate]]+(1 - Table13[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2997,22 +3665,22 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="5">
         <f>IF(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]=0,"N/A",Table13[[#This Row],[True Positive]]/(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="5">
         <f>Table13[[#This Row],[False Positive]]/(Table13[[#This Row],[False Positive]]+Table13[[#This Row],[True Negative]])</f>
         <v>0.5</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="5">
         <f>(Table13[[#This Row],[True Posistive Rate]]+(1 - Table13[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -3027,22 +3695,22 @@
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="5">
         <f>IF(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]=0,"N/A",Table13[[#This Row],[True Positive]]/(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="5">
         <f>Table13[[#This Row],[False Positive]]/(Table13[[#This Row],[False Positive]]+Table13[[#This Row],[True Negative]])</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="5">
         <f>(Table13[[#This Row],[True Posistive Rate]]+(1 - Table13[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0.33333333333333348</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -3057,57 +3725,57 @@
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="5">
         <f>IF(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]=0,"N/A",Table13[[#This Row],[True Positive]]/(Table13[[#This Row],[True Positive]]+Table13[[#This Row],[False Negative]]))</f>
         <v>1</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H36" s="5">
         <f>Table13[[#This Row],[False Positive]]/(Table13[[#This Row],[False Positive]]+Table13[[#This Row],[True Negative]])</f>
         <v>0.5</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="5">
         <f>(Table13[[#This Row],[True Posistive Rate]]+(1 - Table13[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" s="8">
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="7">
         <f t="shared" ref="B37:E37" si="7">SUM(B30:B36)</f>
         <v>17</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <f>SUM(C30:C36)</f>
         <v>1</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="7">
         <f>SUM(D30:D36)</f>
         <v>9</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="7">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="7">
         <f>SUM(F30:F36)</f>
         <v>34</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G37" s="7">
         <f>AVERAGE(G30:G36)</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="7">
         <f t="shared" ref="H37" si="8">AVERAGE(H30:H36)</f>
         <v>0.40476190476190471</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="7">
         <f>ROUND(AVERAGE(I30:I36) * 100, 0)</f>
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A28:I28"/>
@@ -3130,22 +3798,22 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -3161,35 +3829,35 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>93</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>94</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>95</v>
-      </c>
-      <c r="I2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>5</v>
       </c>
       <c r="D3">
@@ -3199,24 +3867,24 @@
         <f t="shared" ref="F3:F9" si="0">SUM(B3:E3)</f>
         <v>7</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <f>IF(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]=0,"N/A",Table1364[[#This Row],[True Positive]]/(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f>Table1364[[#This Row],[False Positive]]/(Table1364[[#This Row],[False Positive]]+Table1364[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <f>(Table1364[[#This Row],[True Posistive Rate]]+(1 - Table1364[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="5">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4">
@@ -3229,24 +3897,24 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f>IF(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]=0,"N/A",Table1364[[#This Row],[True Positive]]/(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <f>Table1364[[#This Row],[False Positive]]/(Table1364[[#This Row],[False Positive]]+Table1364[[#This Row],[True Negative]])</f>
         <v>0.5</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <f>(Table1364[[#This Row],[True Posistive Rate]]+(1 - Table1364[[#This Row],[False Positive Rate]])) - 1</f>
         <v>-0.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="4">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3">
         <v>5</v>
       </c>
       <c r="D5">
@@ -3256,22 +3924,22 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f>IF(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]=0,"N/A",Table1364[[#This Row],[True Positive]]/(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f>Table1364[[#This Row],[False Positive]]/(Table1364[[#This Row],[False Positive]]+Table1364[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <f>(Table1364[[#This Row],[True Posistive Rate]]+(1 - Table1364[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -3283,24 +3951,24 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f>IF(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]=0,"N/A",Table1364[[#This Row],[True Positive]]/(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f>Table1364[[#This Row],[False Positive]]/(Table1364[[#This Row],[False Positive]]+Table1364[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <f>(Table1364[[#This Row],[True Posistive Rate]]+(1 - Table1364[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="4">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7">
@@ -3310,24 +3978,24 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f>IF(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]=0,"N/A",Table1364[[#This Row],[True Positive]]/(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f>Table1364[[#This Row],[False Positive]]/(Table1364[[#This Row],[False Positive]]+Table1364[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <f>(Table1364[[#This Row],[True Posistive Rate]]+(1 - Table1364[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="5">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4">
         <v>3</v>
       </c>
       <c r="D8">
@@ -3337,24 +4005,24 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f>IF(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]=0,"N/A",Table1364[[#This Row],[True Positive]]/(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f>Table1364[[#This Row],[False Positive]]/(Table1364[[#This Row],[False Positive]]+Table1364[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <f>(Table1364[[#This Row],[True Posistive Rate]]+(1 - Table1364[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="4">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3">
         <v>3</v>
       </c>
       <c r="D9">
@@ -3364,57 +4032,57 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f>IF(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]=0,"N/A",Table1364[[#This Row],[True Positive]]/(Table1364[[#This Row],[True Positive]]+Table1364[[#This Row],[False Negative]]))</f>
         <v>0</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f>Table1364[[#This Row],[False Positive]]/(Table1364[[#This Row],[False Positive]]+Table1364[[#This Row],[True Negative]])</f>
         <v>0</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <f>(Table1364[[#This Row],[True Posistive Rate]]+(1 - Table1364[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="8">
+    <row r="10" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="7">
         <f t="shared" ref="B10:E10" si="1">SUM(B3:B9)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <f>SUM(F3:F9)</f>
         <v>34</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f>AVERAGE(G3:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" ref="H10" si="2">AVERAGE(H3:H9)</f>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <f>ROUND(AVERAGE(I3:I9)*100, 0)</f>
         <v>-7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" ht="15.95" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>

<commit_message>
Add all new test cases on Web sheet
</commit_message>
<xml_diff>
--- a/xxetest/Java XXE Test Case Results.xlsx
+++ b/xxetest/Java XXE Test Case Results.xlsx
@@ -7,9 +7,10 @@
     <workbookView xWindow="780" yWindow="465" windowWidth="24825" windowHeight="15540"/>
   </bookViews>
   <sheets>
-    <sheet name="Java XXE Unit Tests" sheetId="1" r:id="rId1"/>
-    <sheet name="Fortify Results" sheetId="2" r:id="rId2"/>
-    <sheet name="Contrast Results" sheetId="3" r:id="rId3"/>
+    <sheet name="Command Line Tests" sheetId="1" r:id="rId1"/>
+    <sheet name="Web Tests" sheetId="4" r:id="rId2"/>
+    <sheet name="Fortify Results" sheetId="2" r:id="rId3"/>
+    <sheet name="Contrast Results" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="186">
   <si>
     <t>Filename</t>
   </si>
@@ -256,9 +257,6 @@
     <t>Proves that enabling validation for the DocumentBuilderFactory leaves the DocumentBuilder unsafe</t>
   </si>
   <si>
-    <t>Proves that XML deserialized using a JAXB Unmarshaller is unsafe when unmarshalled directly from File (Safe in 1.8)</t>
-  </si>
-  <si>
     <t>Proves that XML deserialized using a JAXB Unmarshaller is unsafe when unmarshalled through an XMLStreamReader from an unsafe XMLInputFactory</t>
   </si>
   <si>
@@ -289,28 +287,13 @@
     <t>Proves that SchemaFactory is unsafe by default</t>
   </si>
   <si>
-    <t>Proves that setting SchemaFactory's ACCESS_EXTERNAL_DTD and ACCESS_EXTERNAL_SCHEMA properties makes the Validator safe</t>
-  </si>
-  <si>
     <t>Proves that TransformerFactory is unsafe by default</t>
   </si>
   <si>
     <t>Proves that disabling support for DTD in an XMLInputFactory and then transforming the XML through a safe reader from the XMLInputFactory is safe</t>
   </si>
   <si>
-    <t>Proves that setting TransformerFactory's ACCESS_EXTERNAL_DTD attribute to null makes the Transformer safe in Java 1.8</t>
-  </si>
-  <si>
-    <t>Proves that TransformerFactory has the ACCESS_EXTERNAL_DTD and ACCESS_EXTERNAL_STYLESHEET attributes in Java 1.8 and that they can be set to null</t>
-  </si>
-  <si>
     <t>Proves that XMLInputFactory is unsafe by default</t>
-  </si>
-  <si>
-    <t>Proves that setting XMLInputFactory's ACCESS_EXTERNAL_DTD attribute to null makes the XMLStreamReader safe in Java 1.8</t>
-  </si>
-  <si>
-    <t>Proves that XMLInputFactory has the ACCESS_EXTERNAL_DTD and ACCESS_EXTERNAL_STYLESHEET attributes in Java 1.8 and that they can be set to null</t>
   </si>
   <si>
     <t>Proves that setting XMLInputFactory's IS_SUPPORTING_EXTERNAL_ENTITIES attribute to false makes the XMLStreamReader safe</t>
@@ -375,9 +358,6 @@
     <t>testSafeXMLUsingValidator()</t>
   </si>
   <si>
-    <t>Proves that setting Validator's ACCESS_EXTERNAL_DTD and ACCESS_EXTERNAL_SCHEMA properties makes the Validator safe</t>
-  </si>
-  <si>
     <t>True Positive</t>
   </si>
   <si>
@@ -420,26 +400,425 @@
     <t>Contrast Detection</t>
   </si>
   <si>
-    <t>javax.xml.parsers.DocumentBuilder</t>
-  </si>
-  <si>
-    <t>Unsafe (Safe in 1.8)</t>
-  </si>
-  <si>
-    <t>Fail (Pass in 1.8)</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Proves that setting SchemaFactory's ACCESS_EXTERNAL_DTD and ACCESS_EXTERNAL_SCHEMA properties makes the Validator safe in Java 7u40 and up</t>
+  </si>
+  <si>
+    <t>Proves that setting Validator's ACCESS_EXTERNAL_DTD and ACCESS_EXTERNAL_SCHEMA properties makes the Validator safe in Java 7u40 and up</t>
+  </si>
+  <si>
+    <t>Proves that setting TransformerFactory's ACCESS_EXTERNAL_DTD attribute to null makes the Transformer safe in Java 7u40 and up</t>
+  </si>
+  <si>
+    <t>Proves that TransformerFactory has the ACCESS_EXTERNAL_DTD and ACCESS_EXTERNAL_STYLESHEET attributes in Java 7u40 and up and that they can be set to null</t>
+  </si>
+  <si>
+    <t>Proves that setting XMLInputFactory's ACCESS_EXTERNAL_DTD attribute to null makes the XMLStreamReader safe in Java 7u40 and up</t>
+  </si>
+  <si>
+    <t>Proves that XMLInputFactory has the ACCESS_EXTERNAL_DTD and ACCESS_EXTERNAL_STYLESHEET attributes in Java 7u40 and up and that they can be set to null</t>
+  </si>
+  <si>
+    <t>Results.java</t>
+  </si>
+  <si>
+    <t>Case String</t>
+  </si>
+  <si>
+    <t>documentbuilderunsafedefault</t>
+  </si>
+  <si>
+    <t>documentbuildersafeexpansion</t>
+  </si>
+  <si>
+    <t>documentbuildersafedoctype</t>
+  </si>
+  <si>
+    <t>documentbuildersafeexternal</t>
+  </si>
+  <si>
+    <t>documentbuilderunsafeexternal</t>
+  </si>
+  <si>
+    <t>jaxbunsafefile</t>
+  </si>
+  <si>
+    <t>jaxbunsafeinputfactory</t>
+  </si>
+  <si>
+    <t>jaxbsafefilexmlinputfactory</t>
+  </si>
+  <si>
+    <t>saxunsafedefault</t>
+  </si>
+  <si>
+    <t>saxsafedoctype</t>
+  </si>
+  <si>
+    <t>saxunsafedoctype</t>
+  </si>
+  <si>
+    <t>saxsafeexternal</t>
+  </si>
+  <si>
+    <t>saxunsafeexternal</t>
+  </si>
+  <si>
+    <t>saxunsafevalidationoff</t>
+  </si>
+  <si>
+    <t>documentbuilderunsafevalidationoff</t>
+  </si>
+  <si>
+    <t>documentbuilderunsafevalidationon</t>
+  </si>
+  <si>
+    <t>saxunsafevalidationon</t>
+  </si>
+  <si>
+    <t>schemaunsafe</t>
+  </si>
+  <si>
+    <t>schemasafeaccess</t>
+  </si>
+  <si>
+    <t>schemasafeaccessvalidator</t>
+  </si>
+  <si>
+    <t>transformerunsafedefault</t>
+  </si>
+  <si>
+    <t>transformersafedtd</t>
+  </si>
+  <si>
+    <t>transformersafeaccess</t>
+  </si>
+  <si>
+    <r>
+      <t>java.beans.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XMLDecoder</t>
+    </r>
+  </si>
+  <si>
+    <t>XMLQueryResults.java</t>
+  </si>
+  <si>
+    <t>xmldecoder</t>
+  </si>
+  <si>
+    <t>Unsafe (Safe in 1.8 and up)</t>
+  </si>
+  <si>
+    <t>Fail (Pass in 1.8 and up)</t>
+  </si>
+  <si>
+    <t>Unsafe (Safe in 1.7u51 and up)</t>
+  </si>
+  <si>
+    <t>Proves that XML deserialized using a JAXB Unmarshaller is unsafe when unmarshalled directly from File (Safe in 1.8 and up)</t>
+  </si>
+  <si>
+    <t>Proves that XMLDecoder parses entities in Java versions 1.7u45 and earlier and does not in Java versions 1.7u51 and later</t>
+  </si>
+  <si>
+    <t>Proves that XOM's built in methods do not have the ability to add an external entity reference</t>
+  </si>
+  <si>
+    <r>
+      <t>nu.xom.Document (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XOM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>javax.xml.parsers.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C6500"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DocumentBuilder</t>
+    </r>
+  </si>
+  <si>
+    <t>xmlinputunsafedefault</t>
+  </si>
+  <si>
+    <t>xmlinputsafeaccess</t>
+  </si>
+  <si>
+    <t>xmlinputsafeexternal</t>
+  </si>
+  <si>
+    <t>xmlinputsafedtd</t>
+  </si>
+  <si>
+    <t>xmlinputunsafevalidationoff</t>
+  </si>
+  <si>
+    <t>xmlinputunsafevalidationon</t>
+  </si>
+  <si>
+    <t>xmlreaderunsafedefault</t>
+  </si>
+  <si>
+    <t>xmlreadersafedoctype</t>
+  </si>
+  <si>
+    <t>xmlreaderunsafedoctype</t>
+  </si>
+  <si>
+    <t>xmlreadersafeexternal</t>
+  </si>
+  <si>
+    <t>xmlreaderunsafeexternal</t>
+  </si>
+  <si>
+    <t>xomsafe</t>
+  </si>
+  <si>
+    <t>xomunsafeinputstream</t>
+  </si>
+  <si>
+    <t>xomunsafexmlreader</t>
+  </si>
+  <si>
+    <t>Proves that when building the XOM Document from an unsafe XML InputStream, the Document parses the DTD</t>
+  </si>
+  <si>
+    <t>Proves that when building the XOM Document from an unsafe XMLReader, the Document parses the DTD</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Vulnerability</t>
+  </si>
+  <si>
+    <t>XXE Injection</t>
+  </si>
+  <si>
+    <t>XPath Injection</t>
+  </si>
+  <si>
+    <t>XQuery Injection</t>
+  </si>
+  <si>
+    <r>
+      <t>javax.xml.xpath (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Java XPath API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>org.apache.xalan (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apache Xalan-Java</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>javax.xml.xquery (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Java XQuery API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>xpathunsafeconcat</t>
+  </si>
+  <si>
+    <t>xpathunsafeplaceholder</t>
+  </si>
+  <si>
+    <t>xpathsafeparam</t>
+  </si>
+  <si>
+    <t>xpathsafeescape</t>
+  </si>
+  <si>
+    <t>xalanunsafeconcat</t>
+  </si>
+  <si>
+    <t>xalanunsafeplaceholder</t>
+  </si>
+  <si>
+    <t>xalansafeescape</t>
+  </si>
+  <si>
+    <t>Proves that XPath is vulnerable to injection when using string concatenation on the XPathExpression</t>
+  </si>
+  <si>
+    <t>Proves that XPath is vulnerable to injection when using string placeholders on the XPathExpression</t>
+  </si>
+  <si>
+    <t>Proves that XPath is safe from injection when using an XPathVariableResolver to parameterize the XPathExpression</t>
+  </si>
+  <si>
+    <t>Proves that XPath is safe from injection when using string concatenation while escaping apostrophes on the XPathExpression</t>
+  </si>
+  <si>
+    <t>Proves that Xalan is vulnerable to injection when using string concatenation on the XPath expression</t>
+  </si>
+  <si>
+    <t>Proves that Xalan is vulnerable to injection when using string placeholders on the XPath expression</t>
+  </si>
+  <si>
+    <r>
+      <t>net.sf.saxon.s9api (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Saxonica Saxon9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>saxonunsafeconcat</t>
+  </si>
+  <si>
+    <t>saxonunsafeplaceholder</t>
+  </si>
+  <si>
+    <t>saxonsafeparam</t>
+  </si>
+  <si>
+    <t>saxonsafeescape</t>
+  </si>
+  <si>
+    <t>Proves that Saxon is vulnerable to injection when using string concatenation on the XPath expression</t>
+  </si>
+  <si>
+    <t>Proves that Saxon is vulnerable to injection when using string placeholders on the XPath expression</t>
+  </si>
+  <si>
+    <t>Proves that Saxon is safe from injection when using string concatenation while escaping apostrophes on the XPath expression</t>
+  </si>
+  <si>
+    <t>Proves that XPath is safe from injection when using string concatenation while escaping apostrophes on the XPath expression</t>
+  </si>
+  <si>
+    <t>Proves that Saxon is safe from injection when using a QName to parameterize the XPath expression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,6 +841,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -513,7 +900,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -525,24 +912,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="36">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -588,21 +977,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -648,21 +1037,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -688,21 +1067,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -728,21 +1097,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -768,21 +1127,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -808,151 +1157,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1117,11 +1326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43966464"/>
-        <c:axId val="43967040"/>
+        <c:axId val="42655744"/>
+        <c:axId val="42656320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43966464"/>
+        <c:axId val="42655744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1151,20 +1360,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43967040"/>
+        <c:crossAx val="42656320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43967040"/>
+        <c:axId val="42656320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1189,14 +1397,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43966464"/>
+        <c:crossAx val="42655744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1329,11 +1536,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43968768"/>
-        <c:axId val="43969344"/>
+        <c:axId val="42658048"/>
+        <c:axId val="42658624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43968768"/>
+        <c:axId val="42658048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1363,20 +1570,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43969344"/>
+        <c:crossAx val="42658624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43969344"/>
+        <c:axId val="42658624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1401,14 +1607,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43968768"/>
+        <c:crossAx val="42658048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1541,11 +1746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43971648"/>
-        <c:axId val="43972224"/>
+        <c:axId val="42660928"/>
+        <c:axId val="42661504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43971648"/>
+        <c:axId val="42660928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1575,20 +1780,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43972224"/>
+        <c:crossAx val="42661504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43972224"/>
+        <c:axId val="42661504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1613,14 +1817,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43971648"/>
+        <c:crossAx val="42660928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1760,6 +1963,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:I51">
+  <autoFilter ref="A1:I51"/>
+  <tableColumns count="9">
+    <tableColumn id="8" name="Tests"/>
+    <tableColumn id="3" name="XML Parser" totalsRowLabel="Total"/>
+    <tableColumn id="9" name="Vulnerability"/>
+    <tableColumn id="1" name="Filename"/>
+    <tableColumn id="6" name="Case String"/>
+    <tableColumn id="5" name="Testing if…"/>
+    <tableColumn id="4" name="Fortify Detection"/>
+    <tableColumn id="7" name="Contrast Detection"/>
+    <tableColumn id="2" name="Test Description" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A29:I37">
   <autoFilter ref="A29:I37"/>
   <tableColumns count="9">
@@ -1768,16 +1989,16 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="53"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="52"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="51"/>
-    <tableColumn id="9" name="Score" dataDxfId="50"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="35"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="34"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="33"/>
+    <tableColumn id="9" name="Score" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table136" displayName="Table136" ref="A2:I10">
   <autoFilter ref="A2:I10"/>
   <tableColumns count="9">
@@ -1786,16 +2007,16 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="49"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="48"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="47"/>
-    <tableColumn id="9" name="Score" dataDxfId="46"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="31"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="30"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="29"/>
+    <tableColumn id="9" name="Score" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1364" displayName="Table1364" ref="A2:I10">
   <autoFilter ref="A2:I10"/>
   <tableColumns count="9">
@@ -1804,10 +2025,10 @@
     <tableColumn id="5" name="False Negative"/>
     <tableColumn id="7" name="True Negative"/>
     <tableColumn id="6" name="False Positive"/>
-    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="45"/>
-    <tableColumn id="4" name="True Posistive Rate" dataDxfId="44"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="43"/>
-    <tableColumn id="9" name="Score" dataDxfId="42"/>
+    <tableColumn id="2" name="Total" totalsRowFunction="count" dataDxfId="27"/>
+    <tableColumn id="4" name="True Posistive Rate" dataDxfId="26"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="25"/>
+    <tableColumn id="9" name="Score" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2104,7 +2325,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,14 +2334,14 @@
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="141.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -2135,10 +2356,10 @@
         <v>23</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -2146,7 +2367,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -2161,10 +2382,10 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
         <v>46</v>
@@ -2172,7 +2393,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -2187,10 +2408,10 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
         <v>47</v>
@@ -2198,7 +2419,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -2213,10 +2434,10 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
         <v>48</v>
@@ -2239,38 +2460,38 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="F6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2291,10 +2512,10 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>106</v>
+        <v>96</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="H7" t="s">
         <v>51</v>
@@ -2317,10 +2538,10 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>106</v>
+        <v>95</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="H8" t="s">
         <v>52</v>
@@ -2343,10 +2564,10 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H9" t="s">
         <v>53</v>
@@ -2369,10 +2590,10 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H10" t="s">
         <v>54</v>
@@ -2395,10 +2616,10 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H11" t="s">
         <v>55</v>
@@ -2418,16 +2639,16 @@
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="G12" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2447,13 +2668,13 @@
         <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2473,13 +2694,13 @@
         <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2499,13 +2720,13 @@
         <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2525,13 +2746,13 @@
         <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2551,13 +2772,13 @@
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G17" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2577,13 +2798,13 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G18" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2603,13 +2824,13 @@
         <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2629,13 +2850,13 @@
         <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2655,13 +2876,13 @@
         <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2669,7 +2890,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -2681,13 +2902,13 @@
         <v>21</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2695,7 +2916,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -2707,13 +2928,13 @@
         <v>22</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2721,25 +2942,25 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G24" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2747,7 +2968,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -2759,13 +2980,13 @@
         <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G25" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2773,7 +2994,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -2785,13 +3006,13 @@
         <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G26" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2799,7 +3020,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -2811,21 +3032,21 @@
         <v>22</v>
       </c>
       <c r="F27" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G27" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H27" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -2837,13 +3058,13 @@
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G28" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H28" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2863,13 +3084,13 @@
         <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G29" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2889,18 +3110,18 @@
         <v>22</v>
       </c>
       <c r="F30" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G30" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H30" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>44</v>
@@ -2915,13 +3136,13 @@
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G31" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H31" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2941,13 +3162,13 @@
         <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G32" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2967,13 +3188,13 @@
         <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G33" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2993,13 +3214,13 @@
         <v>21</v>
       </c>
       <c r="F34" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G34" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H34" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3019,13 +3240,13 @@
         <v>22</v>
       </c>
       <c r="F35" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G35" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H35" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3045,13 +3266,13 @@
         <v>21</v>
       </c>
       <c r="F36" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G36" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H36" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3071,13 +3292,13 @@
         <v>22</v>
       </c>
       <c r="F37" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G37" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H37" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3097,13 +3318,13 @@
         <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G38" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H38" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3123,13 +3344,13 @@
         <v>22</v>
       </c>
       <c r="F39" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G39" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H39" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3149,30 +3370,38 @@
         <v>21</v>
       </c>
       <c r="F40" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G40" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="H40" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="Unsafe (Safe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe (Safe",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Unsafe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="Unsafe">
-      <formula>NOT(ISERROR(SEARCH("Unsafe",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Fail (Pass">
+      <formula>NOT(ISERROR(SEARCH("Fail (Pass",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3184,6 +3413,1440 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="141.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" t="s">
+        <v>133</v>
+      </c>
+      <c r="I25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" t="s">
+        <v>95</v>
+      </c>
+      <c r="I26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" t="s">
+        <v>140</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" t="s">
+        <v>95</v>
+      </c>
+      <c r="I29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" t="s">
+        <v>96</v>
+      </c>
+      <c r="H30" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>142</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" t="s">
+        <v>147</v>
+      </c>
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" t="s">
+        <v>95</v>
+      </c>
+      <c r="I34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H35" t="s">
+        <v>96</v>
+      </c>
+      <c r="I35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" t="s">
+        <v>95</v>
+      </c>
+      <c r="I36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" t="s">
+        <v>150</v>
+      </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" t="s">
+        <v>163</v>
+      </c>
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" t="s">
+        <v>164</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" t="s">
+        <v>165</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" t="s">
+        <v>129</v>
+      </c>
+      <c r="E43" t="s">
+        <v>166</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" t="s">
+        <v>167</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" t="s">
+        <v>129</v>
+      </c>
+      <c r="E45" t="s">
+        <v>168</v>
+      </c>
+      <c r="F45" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" t="s">
+        <v>129</v>
+      </c>
+      <c r="E46" t="s">
+        <v>169</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" t="s">
+        <v>177</v>
+      </c>
+      <c r="F47" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" t="s">
+        <v>129</v>
+      </c>
+      <c r="E48" t="s">
+        <v>178</v>
+      </c>
+      <c r="F48" t="s">
+        <v>21</v>
+      </c>
+      <c r="I48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" t="s">
+        <v>179</v>
+      </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" t="s">
+        <v>129</v>
+      </c>
+      <c r="E50" t="s">
+        <v>180</v>
+      </c>
+      <c r="F50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E52:E1048576 F1:F51">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Unsafe (Safe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe (Safe",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Unsafe">
+      <formula>NOT(ISERROR(SEARCH("Unsafe",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Safe">
+      <formula>NOT(ISERROR(SEARCH("Safe",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52:G1048576 G1:H51">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52:G1048576 G1:H51">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Fail (Pass">
+      <formula>NOT(ISERROR(SEARCH("Fail (Pass",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
@@ -3209,45 +4872,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="A1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
         <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3342,7 +5005,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -3369,7 +5032,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3456,7 +5119,7 @@
     </row>
     <row r="10" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B10" s="7">
         <f t="shared" ref="B10" si="1">SUM(B3:B9)</f>
@@ -3493,45 +5156,45 @@
     </row>
     <row r="11" spans="1:9" ht="15.95" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
+      <c r="A28" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I29" t="s">
         <v>88</v>
-      </c>
-      <c r="C29" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" t="s">
-        <v>92</v>
-      </c>
-      <c r="G29" t="s">
-        <v>93</v>
-      </c>
-      <c r="H29" t="s">
-        <v>94</v>
-      </c>
-      <c r="I29" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3623,7 +5286,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -3650,7 +5313,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3740,7 +5403,7 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B37" s="7">
         <f t="shared" ref="B37:E37" si="7">SUM(B30:B36)</f>
@@ -3790,7 +5453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -3812,45 +5475,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="A1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
         <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3939,7 +5602,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -3966,7 +5629,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -4047,7 +5710,7 @@
     </row>
     <row r="10" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B10" s="7">
         <f t="shared" ref="B10:E10" si="1">SUM(B3:B9)</f>

</xml_diff>